<commit_message>
Atualização automática de preços de eletricidade
</commit_message>
<xml_diff>
--- a/output/spot_price_dailyHour_PT.xlsx
+++ b/output/spot_price_dailyHour_PT.xlsx
@@ -652,46 +652,46 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>45871</v>
+        <v>45872</v>
       </c>
       <c r="B2" t="n">
-        <v>97.8</v>
+        <v>80.40000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>77.08</v>
+        <v>69.26000000000001</v>
       </c>
       <c r="D2" t="n">
-        <v>65.27</v>
+        <v>42.96</v>
       </c>
       <c r="E2" t="n">
-        <v>49.56</v>
+        <v>37.38</v>
       </c>
       <c r="F2" t="n">
-        <v>43.33</v>
+        <v>30.02</v>
       </c>
       <c r="G2" t="n">
-        <v>44.29</v>
+        <v>30.2</v>
       </c>
       <c r="H2" t="n">
-        <v>51.08</v>
+        <v>32.03</v>
       </c>
       <c r="I2" t="n">
-        <v>49.81</v>
+        <v>26.28</v>
       </c>
       <c r="J2" t="n">
-        <v>37.33</v>
+        <v>6.16</v>
       </c>
       <c r="K2" t="n">
-        <v>3.52</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>1.06</v>
+        <v>-1.01</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>-2.1</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
@@ -700,34 +700,34 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-1.2</v>
+      </c>
+      <c r="S2" t="n">
         <v>0</v>
       </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.65</v>
-      </c>
       <c r="T2" t="n">
-        <v>4.31</v>
+        <v>0.05</v>
       </c>
       <c r="U2" t="n">
-        <v>15.2</v>
+        <v>27.08</v>
       </c>
       <c r="V2" t="n">
-        <v>74.53</v>
+        <v>78.2</v>
       </c>
       <c r="W2" t="n">
-        <v>99.64</v>
+        <v>96.13</v>
       </c>
       <c r="X2" t="n">
-        <v>99.64</v>
+        <v>97.40000000000001</v>
       </c>
       <c r="Y2" t="n">
-        <v>80.5</v>
+        <v>85.09</v>
       </c>
       <c r="Z2" t="n">
-        <v>37.28</v>
+        <v>30.51</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
@@ -735,7 +735,7 @@
         </is>
       </c>
       <c r="AB2" t="n">
-        <v>88.58</v>
+        <v>89.2</v>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
@@ -743,19 +743,19 @@
         </is>
       </c>
       <c r="AD2" t="n">
-        <v>90.06999999999999</v>
+        <v>91.23999999999999</v>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>0h-2h</t>
+          <t>20h-22h</t>
         </is>
       </c>
       <c r="AF2" t="n">
-        <v>87.44</v>
+        <v>87.16</v>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>9h-19h</t>
+          <t>4h-19h</t>
         </is>
       </c>
     </row>

</xml_diff>